<commit_message>
updated usersAddedStreets to be compatible with current values
</commit_message>
<xml_diff>
--- a/Parser/Train Data/UserAddedStreets.xlsx
+++ b/Parser/Train Data/UserAddedStreets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\SkyDrive\Train Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Transfer\Wispa-Server-Resrouces\Parser\Train Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="582">
   <si>
     <t>Latitude</t>
   </si>
@@ -1755,6 +1755,48 @@
   </si>
   <si>
     <t>Kefar Saba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">נין </t>
+  </si>
+  <si>
+    <t>עדי</t>
+  </si>
+  <si>
+    <t>קלאוזנר</t>
+  </si>
+  <si>
+    <t>יוסף קלאוזנר</t>
+  </si>
+  <si>
+    <t>שם 6</t>
+  </si>
+  <si>
+    <t>שם 7</t>
+  </si>
+  <si>
+    <t>Tel Aviv</t>
+  </si>
+  <si>
+    <t>TLV</t>
+  </si>
+  <si>
+    <t>תל יוסף</t>
+  </si>
+  <si>
+    <t>Tel Yosef</t>
+  </si>
+  <si>
+    <t>Tel Ytzhak</t>
+  </si>
+  <si>
+    <t>תל יצחק</t>
+  </si>
+  <si>
+    <t>תל מונד</t>
+  </si>
+  <si>
+    <t>Tel Mond</t>
   </si>
 </sst>
 </file>
@@ -1863,12 +1905,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A1:I193" totalsRowShown="0">
-  <autoFilter ref="A1:I193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A1:J197" totalsRowShown="0">
+  <autoFilter ref="A1:J197"/>
   <sortState ref="A2:I132">
     <sortCondition ref="A1:A132"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="10">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="מיותר"/>
     <tableColumn id="7" name="שם אב"/>
@@ -1877,15 +1919,16 @@
     <tableColumn id="5" name="שם 3"/>
     <tableColumn id="6" name="שם 4"/>
     <tableColumn id="8" name="שם 5"/>
-    <tableColumn id="9" name="Source"/>
+    <tableColumn id="9" name="שם 6"/>
+    <tableColumn id="10" name="שם 7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A1:B47" tableType="xml" totalsRowShown="0" connectionId="5">
-  <autoFilter ref="A1:B47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A1:B49" tableType="xml" totalsRowShown="0" connectionId="5">
+  <autoFilter ref="A1:B49"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="value" name="מילים לא לחיפוש" dataDxfId="0">
       <xmlColumnPr mapId="6" xpath="/LocationLanguageConfig/ExcludedStrings/ExcludedString/@value" xmlDataType="string"/>
@@ -2173,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView rightToLeft="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2876,10 +2919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I193"/>
+  <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A31" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2892,7 +2935,7 @@
     <col min="7" max="8" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -2918,10 +2961,13 @@
         <v>308</v>
       </c>
       <c r="I1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>572</v>
+      </c>
+      <c r="J1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2946,8 +2992,14 @@
       <c r="H2" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" t="s">
+        <v>574</v>
+      </c>
+      <c r="J2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2964,7 +3016,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2981,7 +3033,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -3004,7 +3056,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -3021,7 +3073,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -3041,7 +3093,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -3058,7 +3110,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -3075,7 +3127,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -3092,7 +3144,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3109,7 +3161,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3126,7 +3178,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -3143,7 +3195,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -3160,7 +3212,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -3177,7 +3229,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -4071,11 +4123,14 @@
       <c r="B68" t="b">
         <v>0</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>19</v>
+      <c r="C68" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" t="s">
+        <v>576</v>
       </c>
       <c r="E68" t="s">
-        <v>20</v>
+        <v>577</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4085,11 +4140,14 @@
       <c r="B69" t="b">
         <v>0</v>
       </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
       <c r="D69" t="s">
-        <v>196</v>
+        <v>579</v>
       </c>
       <c r="E69" t="s">
-        <v>197</v>
+        <v>578</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4099,11 +4157,14 @@
       <c r="B70" t="b">
         <v>0</v>
       </c>
+      <c r="C70" t="s">
+        <v>91</v>
+      </c>
       <c r="D70" t="s">
-        <v>198</v>
+        <v>580</v>
       </c>
       <c r="E70" t="s">
-        <v>199</v>
+        <v>581</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4113,14 +4174,11 @@
       <c r="B71" t="b">
         <v>0</v>
       </c>
-      <c r="D71" t="s">
-        <v>200</v>
+      <c r="D71" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E71" t="s">
-        <v>201</v>
-      </c>
-      <c r="F71" t="s">
-        <v>202</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4131,10 +4189,10 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E72" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4144,11 +4202,11 @@
       <c r="B73" t="b">
         <v>0</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>384</v>
+      <c r="D73" t="s">
+        <v>198</v>
+      </c>
+      <c r="E73" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4159,10 +4217,13 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="E74" t="s">
-        <v>113</v>
+        <v>201</v>
+      </c>
+      <c r="F74" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -4173,13 +4234,10 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E75" t="s">
-        <v>216</v>
-      </c>
-      <c r="F75" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -4189,14 +4247,11 @@
       <c r="B76" t="b">
         <v>0</v>
       </c>
-      <c r="D76" t="s">
-        <v>218</v>
-      </c>
-      <c r="E76" t="s">
-        <v>219</v>
-      </c>
-      <c r="F76" t="s">
-        <v>220</v>
+      <c r="D76" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4207,10 +4262,10 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>223</v>
+        <v>112</v>
       </c>
       <c r="E77" t="s">
-        <v>224</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4221,10 +4276,13 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E78" t="s">
-        <v>226</v>
+        <v>216</v>
+      </c>
+      <c r="F78" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -4235,10 +4293,13 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E79" t="s">
-        <v>228</v>
+        <v>219</v>
+      </c>
+      <c r="F79" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -4249,27 +4310,24 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E80" t="s">
-        <v>230</v>
-      </c>
-      <c r="F80" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B81" t="b">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>58</v>
+        <v>225</v>
       </c>
       <c r="E81" t="s">
-        <v>428</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4280,13 +4338,10 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E82" t="s">
-        <v>235</v>
-      </c>
-      <c r="F82" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4297,27 +4352,27 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E83" t="s">
-        <v>238</v>
+        <v>230</v>
+      </c>
+      <c r="F83" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B84" t="b">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>249</v>
+        <v>58</v>
       </c>
       <c r="E84" t="s">
-        <v>250</v>
-      </c>
-      <c r="F84" t="s">
-        <v>251</v>
+        <v>428</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4327,11 +4382,14 @@
       <c r="B85" t="b">
         <v>0</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>388</v>
+      <c r="D85" t="s">
+        <v>234</v>
+      </c>
+      <c r="E85" t="s">
+        <v>235</v>
+      </c>
+      <c r="F85" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4342,10 +4400,10 @@
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="E86" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4356,10 +4414,13 @@
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E87" t="s">
-        <v>255</v>
+        <v>250</v>
+      </c>
+      <c r="F87" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4369,11 +4430,11 @@
       <c r="B88" t="b">
         <v>0</v>
       </c>
-      <c r="D88" t="s">
-        <v>299</v>
-      </c>
-      <c r="E88" t="s">
-        <v>300</v>
+      <c r="D88" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4384,10 +4445,10 @@
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="E89" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4398,16 +4459,10 @@
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="E90" t="s">
-        <v>267</v>
-      </c>
-      <c r="F90" t="s">
-        <v>268</v>
-      </c>
-      <c r="G90" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4418,10 +4473,10 @@
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>270</v>
+        <v>299</v>
       </c>
       <c r="E91" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4432,10 +4487,10 @@
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E92" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4445,14 +4500,17 @@
       <c r="B93" t="b">
         <v>0</v>
       </c>
-      <c r="C93" t="s">
-        <v>372</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>373</v>
+      <c r="D93" t="s">
+        <v>266</v>
+      </c>
+      <c r="E93" t="s">
+        <v>267</v>
+      </c>
+      <c r="F93" t="s">
+        <v>268</v>
+      </c>
+      <c r="G93" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4463,10 +4521,10 @@
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="E94" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4477,10 +4535,10 @@
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>416</v>
+        <v>272</v>
       </c>
       <c r="E95" t="s">
-        <v>417</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4490,11 +4548,14 @@
       <c r="B96" t="b">
         <v>0</v>
       </c>
-      <c r="D96" t="s">
-        <v>116</v>
-      </c>
-      <c r="E96" t="s">
-        <v>117</v>
+      <c r="C96" t="s">
+        <v>372</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -4505,10 +4566,10 @@
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E97" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4519,13 +4580,10 @@
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>114</v>
+        <v>416</v>
       </c>
       <c r="E98" t="s">
-        <v>115</v>
-      </c>
-      <c r="F98" t="s">
-        <v>326</v>
+        <v>417</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -4535,11 +4593,11 @@
       <c r="B99" t="b">
         <v>0</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>357</v>
+      <c r="D99" t="s">
+        <v>116</v>
+      </c>
+      <c r="E99" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -4550,10 +4608,10 @@
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E100" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4564,10 +4622,13 @@
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>245</v>
+        <v>114</v>
       </c>
       <c r="E101" t="s">
-        <v>246</v>
+        <v>115</v>
+      </c>
+      <c r="F101" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4577,14 +4638,11 @@
       <c r="B102" t="b">
         <v>0</v>
       </c>
-      <c r="D102" t="s">
-        <v>65</v>
-      </c>
-      <c r="E102" t="s">
-        <v>5</v>
-      </c>
-      <c r="F102" t="s">
-        <v>6</v>
+      <c r="D102" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4595,13 +4653,10 @@
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E103" t="s">
-        <v>293</v>
-      </c>
-      <c r="F103" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4611,11 +4666,11 @@
       <c r="B104" t="b">
         <v>0</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>368</v>
+      <c r="D104" t="s">
+        <v>245</v>
+      </c>
+      <c r="E104" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4626,10 +4681,13 @@
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>295</v>
+        <v>65</v>
       </c>
       <c r="E105" t="s">
-        <v>296</v>
+        <v>5</v>
+      </c>
+      <c r="F105" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4640,10 +4698,13 @@
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E106" t="s">
-        <v>298</v>
+        <v>293</v>
+      </c>
+      <c r="F106" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4653,11 +4714,11 @@
       <c r="B107" t="b">
         <v>0</v>
       </c>
-      <c r="D107" t="s">
-        <v>351</v>
-      </c>
-      <c r="E107" t="s">
-        <v>352</v>
+      <c r="D107" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4667,11 +4728,11 @@
       <c r="B108" t="b">
         <v>0</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>394</v>
+      <c r="D108" t="s">
+        <v>295</v>
+      </c>
+      <c r="E108" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4682,10 +4743,10 @@
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="E109" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4696,10 +4757,10 @@
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>306</v>
+        <v>351</v>
       </c>
       <c r="E110" t="s">
-        <v>307</v>
+        <v>352</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4709,11 +4770,11 @@
       <c r="B111" t="b">
         <v>0</v>
       </c>
-      <c r="D111" t="s">
-        <v>148</v>
-      </c>
-      <c r="E111" t="s">
-        <v>149</v>
+      <c r="D111" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4723,14 +4784,11 @@
       <c r="B112" t="b">
         <v>0</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>54</v>
+      <c r="D112" t="s">
+        <v>304</v>
       </c>
       <c r="E112" t="s">
-        <v>55</v>
-      </c>
-      <c r="F112" t="s">
-        <v>142</v>
+        <v>305</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -4740,11 +4798,11 @@
       <c r="B113" t="b">
         <v>0</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>361</v>
+      <c r="D113" t="s">
+        <v>306</v>
+      </c>
+      <c r="E113" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -4754,11 +4812,11 @@
       <c r="B114" t="b">
         <v>0</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>381</v>
+      <c r="D114" t="s">
+        <v>148</v>
+      </c>
+      <c r="E114" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -4769,10 +4827,13 @@
         <v>0</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E115" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="F115" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -4782,11 +4843,11 @@
       <c r="B116" t="b">
         <v>0</v>
       </c>
-      <c r="D116" t="s">
-        <v>209</v>
-      </c>
-      <c r="E116" t="s">
-        <v>210</v>
+      <c r="D116" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -4796,11 +4857,11 @@
       <c r="B117" t="b">
         <v>0</v>
       </c>
-      <c r="D117" t="s">
-        <v>150</v>
-      </c>
-      <c r="E117" t="s">
-        <v>151</v>
+      <c r="D117" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -4811,10 +4872,10 @@
         <v>0</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>412</v>
+        <v>59</v>
+      </c>
+      <c r="E118" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -4825,10 +4886,10 @@
         <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>61</v>
+        <v>209</v>
       </c>
       <c r="E119" t="s">
-        <v>3</v>
+        <v>210</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -4839,13 +4900,10 @@
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>301</v>
+        <v>150</v>
       </c>
       <c r="E120" t="s">
-        <v>302</v>
-      </c>
-      <c r="F120" t="s">
-        <v>303</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -4856,10 +4914,10 @@
         <v>0</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>348</v>
+        <v>411</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>349</v>
+        <v>412</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -4870,10 +4928,10 @@
         <v>0</v>
       </c>
       <c r="D122" t="s">
-        <v>418</v>
+        <v>61</v>
       </c>
       <c r="E122" t="s">
-        <v>419</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4884,10 +4942,13 @@
         <v>0</v>
       </c>
       <c r="D123" t="s">
-        <v>22</v>
+        <v>301</v>
       </c>
       <c r="E123" t="s">
-        <v>23</v>
+        <v>302</v>
+      </c>
+      <c r="F123" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -4897,14 +4958,11 @@
       <c r="B124" t="b">
         <v>0</v>
       </c>
-      <c r="C124" t="s">
-        <v>91</v>
-      </c>
-      <c r="D124" t="s">
-        <v>92</v>
-      </c>
-      <c r="E124" t="s">
-        <v>93</v>
+      <c r="D124" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -4914,11 +4972,11 @@
       <c r="B125" t="b">
         <v>0</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>369</v>
+      <c r="D125" t="s">
+        <v>418</v>
+      </c>
+      <c r="E125" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -4929,10 +4987,10 @@
         <v>0</v>
       </c>
       <c r="D126" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="E126" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -4942,11 +5000,14 @@
       <c r="B127" t="b">
         <v>0</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>370</v>
+      <c r="C127" t="s">
+        <v>91</v>
+      </c>
+      <c r="D127" t="s">
+        <v>92</v>
+      </c>
+      <c r="E127" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -4957,10 +5018,10 @@
         <v>0</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E128" t="s">
-        <v>30</v>
+        <v>313</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -4970,11 +5031,11 @@
       <c r="B129" t="b">
         <v>0</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>371</v>
+      <c r="D129" t="s">
+        <v>66</v>
+      </c>
+      <c r="E129" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4985,10 +5046,10 @@
         <v>0</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>399</v>
+        <v>314</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>400</v>
+        <v>370</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -4999,10 +5060,10 @@
         <v>0</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="E131" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -5012,11 +5073,11 @@
       <c r="B132" t="b">
         <v>0</v>
       </c>
-      <c r="D132" t="s">
-        <v>243</v>
-      </c>
-      <c r="E132" t="s">
-        <v>244</v>
+      <c r="D132" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -5026,11 +5087,11 @@
       <c r="B133" t="b">
         <v>0</v>
       </c>
-      <c r="D133" t="s">
-        <v>194</v>
-      </c>
-      <c r="E133" t="s">
-        <v>195</v>
+      <c r="D133" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -5040,14 +5101,11 @@
       <c r="B134" t="b">
         <v>0</v>
       </c>
-      <c r="C134" t="s">
-        <v>372</v>
-      </c>
       <c r="D134" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>415</v>
+        <v>56</v>
+      </c>
+      <c r="E134" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -5058,10 +5116,10 @@
         <v>0</v>
       </c>
       <c r="D135" t="s">
-        <v>21</v>
+        <v>243</v>
       </c>
       <c r="E135" t="s">
-        <v>99</v>
+        <v>244</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -5071,14 +5129,11 @@
       <c r="B136" t="b">
         <v>0</v>
       </c>
-      <c r="C136" t="s">
-        <v>50</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>366</v>
+      <c r="D136" t="s">
+        <v>194</v>
+      </c>
+      <c r="E136" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -5088,11 +5143,14 @@
       <c r="B137" t="b">
         <v>0</v>
       </c>
+      <c r="C137" t="s">
+        <v>372</v>
+      </c>
       <c r="D137" s="1" t="s">
-        <v>311</v>
+        <v>350</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>367</v>
+        <v>415</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -5103,10 +5161,13 @@
         <v>0</v>
       </c>
       <c r="D138" t="s">
-        <v>211</v>
+        <v>21</v>
       </c>
       <c r="E138" t="s">
-        <v>212</v>
+        <v>99</v>
+      </c>
+      <c r="F138" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -5116,17 +5177,14 @@
       <c r="B139" t="b">
         <v>0</v>
       </c>
-      <c r="D139" t="s">
-        <v>51</v>
-      </c>
-      <c r="E139" t="s">
-        <v>53</v>
-      </c>
-      <c r="F139" t="s">
-        <v>52</v>
-      </c>
-      <c r="G139" t="s">
-        <v>442</v>
+      <c r="C139" t="s">
+        <v>50</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -5136,11 +5194,11 @@
       <c r="B140" t="b">
         <v>0</v>
       </c>
-      <c r="D140" t="s">
-        <v>213</v>
-      </c>
-      <c r="E140" t="s">
-        <v>214</v>
+      <c r="D140" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -5151,10 +5209,10 @@
         <v>0</v>
       </c>
       <c r="D141" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E141" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -5164,11 +5222,17 @@
       <c r="B142" t="b">
         <v>0</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>354</v>
+      <c r="D142" t="s">
+        <v>51</v>
+      </c>
+      <c r="E142" t="s">
+        <v>53</v>
+      </c>
+      <c r="F142" t="s">
+        <v>52</v>
+      </c>
+      <c r="G142" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -5178,11 +5242,11 @@
       <c r="B143" t="b">
         <v>0</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>379</v>
+      <c r="D143" t="s">
+        <v>213</v>
+      </c>
+      <c r="E143" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -5193,57 +5257,66 @@
         <v>0</v>
       </c>
       <c r="D144" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="E144" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>34</v>
+        <v>353</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B146" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>34</v>
+        <v>378</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B147" t="b">
-        <v>1</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="D147" t="s">
+        <v>239</v>
+      </c>
+      <c r="E147" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B148" t="b">
-        <v>1</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="D148" t="s">
+        <v>570</v>
       </c>
       <c r="E148" t="s">
-        <v>42</v>
+        <v>571</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5254,7 +5327,7 @@
         <v>1</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -5262,13 +5335,10 @@
         <v>106</v>
       </c>
       <c r="B150" t="b">
-        <v>0</v>
-      </c>
-      <c r="D150" t="s">
-        <v>108</v>
-      </c>
-      <c r="E150" t="s">
-        <v>109</v>
+        <v>1</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -5276,10 +5346,10 @@
         <v>106</v>
       </c>
       <c r="B151" t="b">
-        <v>0</v>
-      </c>
-      <c r="D151" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -5287,10 +5357,13 @@
         <v>106</v>
       </c>
       <c r="B152" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="E152" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -5298,10 +5371,10 @@
         <v>106</v>
       </c>
       <c r="B153" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -5309,13 +5382,13 @@
         <v>106</v>
       </c>
       <c r="B154" t="b">
-        <v>1</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="D154" t="s">
+        <v>108</v>
       </c>
       <c r="E154" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -5323,16 +5396,10 @@
         <v>106</v>
       </c>
       <c r="B155" t="b">
-        <v>1</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E155" t="s">
-        <v>43</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
+      </c>
+      <c r="D155" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -5340,13 +5407,10 @@
         <v>106</v>
       </c>
       <c r="B156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E156" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -5354,69 +5418,69 @@
         <v>106</v>
       </c>
       <c r="B157" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B158" t="b">
-        <v>0</v>
-      </c>
-      <c r="D158" t="s">
-        <v>232</v>
+        <v>1</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E158" t="s">
-        <v>233</v>
+        <v>33</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B159" t="b">
-        <v>0</v>
-      </c>
-      <c r="D159" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E159" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B160" t="b">
-        <v>0</v>
-      </c>
-      <c r="D160" t="s">
-        <v>241</v>
+        <v>1</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E160" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B161" t="b">
-        <v>0</v>
-      </c>
-      <c r="D161" t="s">
-        <v>247</v>
-      </c>
-      <c r="E161" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
         <v>107</v>
       </c>
@@ -5424,13 +5488,13 @@
         <v>0</v>
       </c>
       <c r="D162" t="s">
-        <v>323</v>
+        <v>232</v>
       </c>
       <c r="E162" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
         <v>107</v>
       </c>
@@ -5438,13 +5502,13 @@
         <v>0</v>
       </c>
       <c r="D163" t="s">
-        <v>256</v>
+        <v>12</v>
       </c>
       <c r="E163" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>107</v>
       </c>
@@ -5452,13 +5516,13 @@
         <v>0</v>
       </c>
       <c r="D164" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="E164" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
         <v>107</v>
       </c>
@@ -5466,13 +5530,13 @@
         <v>0</v>
       </c>
       <c r="D165" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="E165" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>107</v>
       </c>
@@ -5480,13 +5544,13 @@
         <v>0</v>
       </c>
       <c r="D166" t="s">
-        <v>262</v>
+        <v>323</v>
       </c>
       <c r="E166" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
         <v>107</v>
       </c>
@@ -5494,27 +5558,27 @@
         <v>0</v>
       </c>
       <c r="D167" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="E167" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
         <v>107</v>
       </c>
       <c r="B168" t="b">
         <v>0</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="D168" t="s">
+        <v>258</v>
+      </c>
+      <c r="E168" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
         <v>107</v>
       </c>
@@ -5522,13 +5586,13 @@
         <v>0</v>
       </c>
       <c r="D169" t="s">
-        <v>143</v>
+        <v>260</v>
       </c>
       <c r="E169" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
         <v>107</v>
       </c>
@@ -5536,13 +5600,13 @@
         <v>0</v>
       </c>
       <c r="D170" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="E170" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
         <v>107</v>
       </c>
@@ -5550,27 +5614,27 @@
         <v>0</v>
       </c>
       <c r="D171" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E171" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
         <v>107</v>
       </c>
       <c r="B172" t="b">
         <v>0</v>
       </c>
-      <c r="D172" t="s">
-        <v>280</v>
-      </c>
-      <c r="E172" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6">
+      <c r="D172" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
         <v>107</v>
       </c>
@@ -5578,13 +5642,13 @@
         <v>0</v>
       </c>
       <c r="D173" t="s">
-        <v>284</v>
+        <v>143</v>
       </c>
       <c r="E173" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
         <v>107</v>
       </c>
@@ -5592,13 +5656,13 @@
         <v>0</v>
       </c>
       <c r="D174" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="E174" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
         <v>107</v>
       </c>
@@ -5606,16 +5670,13 @@
         <v>0</v>
       </c>
       <c r="D175" t="s">
-        <v>101</v>
+        <v>278</v>
       </c>
       <c r="E175" t="s">
-        <v>102</v>
-      </c>
-      <c r="F175" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
         <v>107</v>
       </c>
@@ -5623,10 +5684,10 @@
         <v>0</v>
       </c>
       <c r="D176" t="s">
-        <v>186</v>
+        <v>280</v>
       </c>
       <c r="E176" t="s">
-        <v>185</v>
+        <v>281</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5637,10 +5698,10 @@
         <v>0</v>
       </c>
       <c r="D177" t="s">
-        <v>207</v>
+        <v>284</v>
       </c>
       <c r="E177" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5651,10 +5712,10 @@
         <v>0</v>
       </c>
       <c r="D178" t="s">
-        <v>205</v>
+        <v>288</v>
       </c>
       <c r="E178" t="s">
-        <v>206</v>
+        <v>289</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5665,10 +5726,13 @@
         <v>0</v>
       </c>
       <c r="D179" t="s">
-        <v>183</v>
+        <v>101</v>
       </c>
       <c r="E179" t="s">
-        <v>184</v>
+        <v>102</v>
+      </c>
+      <c r="F179" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5679,10 +5743,10 @@
         <v>0</v>
       </c>
       <c r="D180" t="s">
-        <v>413</v>
+        <v>186</v>
       </c>
       <c r="E180" t="s">
-        <v>414</v>
+        <v>185</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5693,10 +5757,10 @@
         <v>0</v>
       </c>
       <c r="D181" t="s">
-        <v>57</v>
+        <v>207</v>
       </c>
       <c r="E181" t="s">
-        <v>110</v>
+        <v>208</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5707,10 +5771,10 @@
         <v>0</v>
       </c>
       <c r="D182" t="s">
-        <v>321</v>
+        <v>205</v>
       </c>
       <c r="E182" t="s">
-        <v>320</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5720,11 +5784,11 @@
       <c r="B183" t="b">
         <v>0</v>
       </c>
-      <c r="D183" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>386</v>
+      <c r="D183" t="s">
+        <v>183</v>
+      </c>
+      <c r="E183" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5735,12 +5799,11 @@
         <v>0</v>
       </c>
       <c r="D184" t="s">
-        <v>318</v>
+        <v>413</v>
       </c>
       <c r="E184" t="s">
-        <v>317</v>
-      </c>
-      <c r="H184" s="2"/>
+        <v>414</v>
+      </c>
     </row>
     <row r="185" spans="1:8">
       <c r="A185" t="s">
@@ -5749,11 +5812,11 @@
       <c r="B185" t="b">
         <v>0</v>
       </c>
-      <c r="D185" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>390</v>
+      <c r="D185" t="s">
+        <v>57</v>
+      </c>
+      <c r="E185" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5763,11 +5826,11 @@
       <c r="B186" t="b">
         <v>0</v>
       </c>
-      <c r="D186" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>330</v>
+      <c r="D186" t="s">
+        <v>321</v>
+      </c>
+      <c r="E186" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5777,11 +5840,11 @@
       <c r="B187" t="b">
         <v>0</v>
       </c>
-      <c r="D187" t="s">
-        <v>420</v>
-      </c>
-      <c r="E187" t="s">
-        <v>421</v>
+      <c r="D187" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5792,14 +5855,12 @@
         <v>0</v>
       </c>
       <c r="D188" t="s">
-        <v>391</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>358</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="E188" t="s">
+        <v>317</v>
+      </c>
+      <c r="H188" s="2"/>
     </row>
     <row r="189" spans="1:8">
       <c r="A189" t="s">
@@ -5808,14 +5869,11 @@
       <c r="B189" t="b">
         <v>0</v>
       </c>
-      <c r="D189" t="s">
-        <v>145</v>
-      </c>
-      <c r="E189" t="s">
-        <v>146</v>
-      </c>
-      <c r="F189" t="s">
-        <v>147</v>
+      <c r="D189" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5825,11 +5883,11 @@
       <c r="B190" t="b">
         <v>0</v>
       </c>
-      <c r="D190" t="s">
-        <v>422</v>
-      </c>
-      <c r="E190" t="s">
-        <v>423</v>
+      <c r="D190" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5840,27 +5898,30 @@
         <v>0</v>
       </c>
       <c r="D191" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="E191" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
     </row>
     <row r="192" spans="1:8">
       <c r="A192" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B192" t="b">
         <v>0</v>
       </c>
       <c r="D192" t="s">
-        <v>434</v>
-      </c>
-      <c r="E192" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5">
+        <v>391</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>107</v>
       </c>
@@ -5868,15 +5929,74 @@
         <v>0</v>
       </c>
       <c r="D193" t="s">
+        <v>145</v>
+      </c>
+      <c r="E193" t="s">
+        <v>146</v>
+      </c>
+      <c r="F193" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" t="s">
+        <v>107</v>
+      </c>
+      <c r="B194" t="b">
+        <v>0</v>
+      </c>
+      <c r="D194" t="s">
+        <v>422</v>
+      </c>
+      <c r="E194" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" t="s">
+        <v>107</v>
+      </c>
+      <c r="B195" t="b">
+        <v>0</v>
+      </c>
+      <c r="D195" t="s">
+        <v>404</v>
+      </c>
+      <c r="E195" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" t="s">
+        <v>124</v>
+      </c>
+      <c r="B196" t="b">
+        <v>0</v>
+      </c>
+      <c r="D196" t="s">
+        <v>434</v>
+      </c>
+      <c r="E196" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" t="s">
+        <v>107</v>
+      </c>
+      <c r="B197" t="b">
+        <v>0</v>
+      </c>
+      <c r="D197" t="s">
         <v>436</v>
       </c>
-      <c r="E193" t="s">
+      <c r="E197" t="s">
         <v>437</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A193 A194:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A197 A198:A1048576">
       <formula1>"Prefix,MainBody,Word"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5916,10 +6036,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6301,6 +6421,22 @@
         <v>432</v>
       </c>
       <c r="B47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B49" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>